<commit_message>
LakeShore 331 support, busy device
</commit_message>
<xml_diff>
--- a/startup/xlsx/lakeshore.xlsx
+++ b/startup/xlsx/lakeshore.xlsx
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="69">
   <si>
     <t xml:space="preserve">LakeShore</t>
   </si>
@@ -184,6 +184,9 @@
     <t xml:space="preserve">Settling time (seconds)</t>
   </si>
   <si>
+    <t xml:space="preserve">Power</t>
+  </si>
+  <si>
     <t xml:space="preserve">Measure this temperature?</t>
   </si>
   <si>
@@ -260,6 +263,9 @@
   </si>
   <si>
     <t xml:space="preserve">CIF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">medium</t>
   </si>
   <si>
     <t xml:space="preserve">best_sample_ever</t>
@@ -338,9 +344,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -400,7 +407,7 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -416,7 +423,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCFF66"/>
-        <bgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCFF660"/>
       </patternFill>
     </fill>
     <fill>
@@ -435,6 +442,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFCCCCCC"/>
         <bgColor rgb="FFE0C2CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFF660"/>
+        <bgColor rgb="FFCCFF66"/>
       </patternFill>
     </fill>
   </fills>
@@ -655,7 +668,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -676,7 +689,11 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -684,7 +701,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -780,7 +797,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -832,15 +853,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -852,7 +873,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -880,15 +901,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -945,7 +966,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFCFF660"/>
       <rgbColor rgb="FFCCFF66"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99FF"/>
@@ -978,14 +999,14 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>416160</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>102240</xdr:rowOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>122760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1137960</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>105480</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>176040</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>125640</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -995,7 +1016,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3192840" y="3926160"/>
-          <a:ext cx="6645600" cy="1791360"/>
+          <a:ext cx="6645960" cy="1791000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1228,9 +1249,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1137960</xdr:colOff>
+      <xdr:colOff>1137600</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>105480</xdr:rowOff>
+      <xdr:rowOff>105120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1240,7 +1261,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3192840" y="3926160"/>
-          <a:ext cx="6645600" cy="1791360"/>
+          <a:ext cx="6645960" cy="1791000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1473,9 +1494,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1137960</xdr:colOff>
+      <xdr:colOff>1137600</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>105480</xdr:rowOff>
+      <xdr:rowOff>105120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1485,7 +1506,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3192840" y="3926160"/>
-          <a:ext cx="6645600" cy="1791360"/>
+          <a:ext cx="6645960" cy="1791000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1712,35 +1733,35 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:AC14"/>
+  <dimension ref="B1:AD14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="6" topLeftCell="D7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="17.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="12.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="10.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="14.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="12" style="0" width="29.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="22.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="26" min="21" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="27" style="0" width="24.87"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="28" style="0" width="27.09"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="29" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="13.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="17.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="14.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="0" width="29.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="22.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="19" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="27" min="22" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="28" min="28" style="0" width="24.87"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="29" min="29" style="0" width="27.09"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="0" width="24.87"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1772,119 +1793,123 @@
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-    </row>
-    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Z1" s="0"/>
+      <c r="AA1" s="4"/>
+    </row>
+    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="5" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
         <v>Version: 8</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="7" t="s">
+      <c r="I2" s="7"/>
+      <c r="J2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="0"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
+      <c r="V2" s="12"/>
       <c r="W2" s="0"/>
       <c r="X2" s="0"/>
       <c r="Y2" s="0"/>
-      <c r="Z2" s="11"/>
+      <c r="Z2" s="0"/>
+      <c r="AA2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
       <c r="U3" s="11"/>
-      <c r="V3" s="0"/>
+      <c r="V3" s="12"/>
       <c r="W3" s="0"/>
       <c r="X3" s="0"/>
       <c r="Y3" s="0"/>
-      <c r="Z3" s="11"/>
+      <c r="Z3" s="0"/>
+      <c r="AA3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="14"/>
+      <c r="G4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="15" t="s">
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="16" t="s">
+      <c r="K4" s="16"/>
+      <c r="L4" s="16"/>
+      <c r="M4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16" t="s">
+      <c r="N4" s="17"/>
+      <c r="O4" s="17"/>
+      <c r="P4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16" t="s">
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16" t="s">
+      <c r="T4" s="17"/>
+      <c r="U4" s="17"/>
+      <c r="V4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="17" t="s">
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="17"/>
+      <c r="AB4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="AB4" s="17"/>
-      <c r="AC4" s="17"/>
+      <c r="AC4" s="18"/>
+      <c r="AD4" s="18"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="19" t="s">
         <v>16</v>
       </c>
       <c r="D5" s="19" t="s">
@@ -1893,16 +1918,16 @@
       <c r="E5" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="F5" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="I5" s="21" t="s">
+      <c r="I5" s="19" t="s">
         <v>22</v>
       </c>
       <c r="J5" s="22" t="s">
@@ -1914,369 +1939,382 @@
       <c r="L5" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="20" t="s">
+      <c r="M5" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="N5" s="25" t="s">
+      <c r="N5" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="O5" s="24" t="s">
+      <c r="O5" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="P5" s="20" t="s">
+      <c r="P5" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="Q5" s="25" t="s">
+      <c r="Q5" s="21" t="s">
         <v>30</v>
       </c>
       <c r="R5" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="S5" s="20" t="s">
+      <c r="S5" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="T5" s="27" t="s">
+      <c r="T5" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="U5" s="19" t="s">
+      <c r="U5" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="V5" s="18" t="s">
+      <c r="V5" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="W5" s="18" t="s">
+      <c r="W5" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="X5" s="18" t="s">
+      <c r="X5" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="Y5" s="18" t="s">
+      <c r="Y5" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="Z5" s="23" t="s">
+      <c r="Z5" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="AA5" s="21" t="s">
+      <c r="AA5" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="AB5" s="28" t="s">
+      <c r="AB5" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="AC5" s="28" t="s">
+      <c r="AC5" s="29" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" s="29" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="30" t="n">
+      <c r="AD5" s="29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" s="30" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="31" t="n">
         <v>15</v>
       </c>
-      <c r="C6" s="30" t="n">
+      <c r="C6" s="31" t="n">
         <v>10</v>
       </c>
-      <c r="D6" s="31" t="s">
+      <c r="D6" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="30" t="n">
+      <c r="F6" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="31" t="n">
         <v>1</v>
       </c>
-      <c r="G6" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="34" t="s">
+      <c r="H6" s="31" t="s">
         <v>46</v>
       </c>
-      <c r="J6" s="35" t="s">
+      <c r="I6" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="36" t="s">
+      <c r="J6" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="L6" s="37" t="s">
+      <c r="K6" s="37" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="L6" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="N6" s="39" t="s">
+      <c r="M6" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="O6" s="40" t="s">
+      <c r="N6" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="P6" s="41" t="s">
+      <c r="O6" s="41" t="s">
         <v>53</v>
       </c>
-      <c r="Q6" s="42" t="s">
+      <c r="P6" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="R6" s="43"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="44" t="n">
+      <c r="Q6" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="R6" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="S6" s="45"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="44"/>
+      <c r="V6" s="46" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="V6" s="45" t="n">
+      <c r="W6" s="47" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="W6" s="45" t="n">
+      <c r="X6" s="47" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="X6" s="45" t="n">
+      <c r="Y6" s="47" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Y6" s="45" t="n">
+      <c r="Z6" s="47" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z6" s="46" t="n">
+      <c r="AA6" s="48" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="47"/>
-      <c r="AB6" s="42"/>
-      <c r="AC6" s="42"/>
+      <c r="AB6" s="49"/>
+      <c r="AC6" s="44"/>
+      <c r="AD6" s="44"/>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="48" t="n">
+      <c r="B7" s="50" t="n">
         <v>15</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="49" t="s">
+      <c r="C7" s="50"/>
+      <c r="E7" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="50"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="54"/>
-      <c r="T7" s="55"/>
-      <c r="U7" s="56"/>
-      <c r="V7" s="57"/>
-      <c r="W7" s="57"/>
-      <c r="X7" s="57"/>
-      <c r="Y7" s="57"/>
-      <c r="Z7" s="58"/>
-      <c r="AA7" s="59"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="13"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="50"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="52"/>
+      <c r="O7" s="56"/>
+      <c r="P7" s="55"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="56"/>
+      <c r="U7" s="57"/>
+      <c r="V7" s="58"/>
+      <c r="W7" s="59"/>
+      <c r="X7" s="59"/>
+      <c r="Y7" s="59"/>
+      <c r="Z7" s="59"/>
+      <c r="AA7" s="60"/>
+      <c r="AB7" s="61"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="48" t="n">
+      <c r="B8" s="50" t="n">
         <v>100</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="49" t="s">
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="50"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="53"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="54"/>
-      <c r="T8" s="55"/>
-      <c r="U8" s="56"/>
-      <c r="V8" s="57"/>
-      <c r="W8" s="57"/>
-      <c r="X8" s="57"/>
-      <c r="Y8" s="57"/>
-      <c r="Z8" s="58"/>
-      <c r="AA8" s="59"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="13"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="54"/>
+      <c r="L8" s="50"/>
+      <c r="M8" s="55"/>
+      <c r="N8" s="52"/>
+      <c r="O8" s="56"/>
+      <c r="P8" s="55"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="56"/>
+      <c r="U8" s="57"/>
+      <c r="V8" s="58"/>
+      <c r="W8" s="59"/>
+      <c r="X8" s="59"/>
+      <c r="Y8" s="59"/>
+      <c r="Z8" s="59"/>
+      <c r="AA8" s="60"/>
+      <c r="AB8" s="61"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="48" t="n">
+      <c r="B9" s="50" t="n">
         <v>150</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="49" t="s">
+      <c r="C9" s="50"/>
+      <c r="D9" s="50"/>
+      <c r="E9" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="53"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="54"/>
-      <c r="T9" s="55"/>
-      <c r="U9" s="56"/>
-      <c r="V9" s="57"/>
-      <c r="W9" s="57"/>
-      <c r="X9" s="57"/>
-      <c r="Y9" s="57"/>
-      <c r="Z9" s="58"/>
-      <c r="AA9" s="59"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="53"/>
+      <c r="K9" s="54"/>
+      <c r="L9" s="50"/>
+      <c r="M9" s="55"/>
+      <c r="N9" s="52"/>
+      <c r="O9" s="56"/>
+      <c r="P9" s="55"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="56"/>
+      <c r="U9" s="57"/>
+      <c r="V9" s="58"/>
+      <c r="W9" s="59"/>
+      <c r="X9" s="59"/>
+      <c r="Y9" s="59"/>
+      <c r="Z9" s="59"/>
+      <c r="AA9" s="60"/>
+      <c r="AB9" s="61"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="48" t="n">
+      <c r="B10" s="50" t="n">
         <v>200</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49" t="s">
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="53"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="54"/>
-      <c r="T10" s="55"/>
-      <c r="U10" s="56"/>
-      <c r="V10" s="57"/>
-      <c r="W10" s="57"/>
-      <c r="X10" s="57"/>
-      <c r="Y10" s="57"/>
-      <c r="Z10" s="58"/>
-      <c r="AA10" s="59"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="53"/>
+      <c r="K10" s="54"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="55"/>
+      <c r="N10" s="52"/>
+      <c r="O10" s="56"/>
+      <c r="P10" s="55"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="56"/>
+      <c r="U10" s="57"/>
+      <c r="V10" s="58"/>
+      <c r="W10" s="59"/>
+      <c r="X10" s="59"/>
+      <c r="Y10" s="59"/>
+      <c r="Z10" s="59"/>
+      <c r="AA10" s="60"/>
+      <c r="AB10" s="61"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="48" t="n">
+      <c r="B11" s="50" t="n">
         <v>250</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="49" t="s">
+      <c r="C11" s="50"/>
+      <c r="D11" s="50"/>
+      <c r="E11" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="53"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="54"/>
-      <c r="T11" s="55"/>
-      <c r="U11" s="56"/>
-      <c r="V11" s="57"/>
-      <c r="W11" s="57"/>
-      <c r="X11" s="57"/>
-      <c r="Y11" s="57"/>
-      <c r="Z11" s="58"/>
-      <c r="AA11" s="59"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="13"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="50"/>
+      <c r="M11" s="55"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="56"/>
+      <c r="P11" s="55"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="56"/>
+      <c r="U11" s="57"/>
+      <c r="V11" s="58"/>
+      <c r="W11" s="59"/>
+      <c r="X11" s="59"/>
+      <c r="Y11" s="59"/>
+      <c r="Z11" s="59"/>
+      <c r="AA11" s="60"/>
+      <c r="AB11" s="61"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="48" t="n">
+      <c r="B12" s="50" t="n">
         <v>300</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="49" t="s">
+      <c r="C12" s="50"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="54"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="54"/>
-      <c r="T12" s="55"/>
-      <c r="U12" s="56"/>
-      <c r="V12" s="57"/>
-      <c r="W12" s="57"/>
-      <c r="X12" s="57"/>
-      <c r="Y12" s="57"/>
-      <c r="Z12" s="58"/>
-      <c r="AA12" s="59"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13"/>
+      <c r="J12" s="53"/>
+      <c r="K12" s="54"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="55"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="56"/>
+      <c r="P12" s="55"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="56"/>
+      <c r="U12" s="57"/>
+      <c r="V12" s="58"/>
+      <c r="W12" s="59"/>
+      <c r="X12" s="59"/>
+      <c r="Y12" s="59"/>
+      <c r="Z12" s="59"/>
+      <c r="AA12" s="60"/>
+      <c r="AB12" s="61"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="48"/>
-      <c r="C13" s="48"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="53"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="54"/>
-      <c r="O13" s="53"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="54"/>
-      <c r="T13" s="55"/>
-      <c r="U13" s="56"/>
-      <c r="V13" s="57"/>
-      <c r="W13" s="57"/>
-      <c r="X13" s="57"/>
-      <c r="Y13" s="57"/>
-      <c r="Z13" s="58"/>
-      <c r="AA13" s="59"/>
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="51"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="13"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="54"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="55"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="56"/>
+      <c r="P13" s="55"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="56"/>
+      <c r="U13" s="57"/>
+      <c r="V13" s="58"/>
+      <c r="W13" s="59"/>
+      <c r="X13" s="59"/>
+      <c r="Y13" s="59"/>
+      <c r="Z13" s="59"/>
+      <c r="AA13" s="60"/>
+      <c r="AB13" s="61"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="48"/>
-      <c r="C14" s="48"/>
-      <c r="D14" s="49"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="53"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="54"/>
-      <c r="T14" s="55"/>
-      <c r="U14" s="56"/>
-      <c r="V14" s="57"/>
-      <c r="W14" s="57"/>
-      <c r="X14" s="57"/>
-      <c r="Y14" s="57"/>
-      <c r="Z14" s="58"/>
-      <c r="AA14" s="59"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="54"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="55"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="56"/>
+      <c r="P14" s="55"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="56"/>
+      <c r="U14" s="57"/>
+      <c r="V14" s="58"/>
+      <c r="W14" s="59"/>
+      <c r="X14" s="59"/>
+      <c r="Y14" s="59"/>
+      <c r="Z14" s="59"/>
+      <c r="AA14" s="60"/>
+      <c r="AB14" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2285,57 +2323,57 @@
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="E2:F2"/>
     <mergeCell ref="H2:I2"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="I4:K4"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:Q4"/>
-    <mergeCell ref="R4:T4"/>
-    <mergeCell ref="U4:Z4"/>
-    <mergeCell ref="AA4:AC4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="S4:U4"/>
+    <mergeCell ref="V4:AA4"/>
+    <mergeCell ref="AB4:AD4"/>
   </mergeCells>
-  <dataValidations count="13">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="U6:Z14" type="list">
+  <dataValidations count="14">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:AA14" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6:J14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6:L14" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F6:F14" type="whole">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G14" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 D6:D14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G2 J2 E6:E14" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AA6:AC6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AB6:AD6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H7:H14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I14" type="list">
       <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:C70" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:C12 B13:D70" type="decimal">
       <formula1>-277</formula1>
       <formula2>500</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J14" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2343,9 +2381,13 @@
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end,Temperature at beginning,Temperature at end,Temperature+element at beginning,Temperature+element at end,Temperature+element+edge at beginning,Temperature+element+edge at "</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="R6:T14" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U14" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D6 D8:D12" type="list">
+      <formula1>"low,medium,high"</formula1>
+      <formula2>500</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2375,7 +2417,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
@@ -2433,511 +2475,511 @@
         <v>Version: 8</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="7" t="s">
+      <c r="I2" s="7"/>
+      <c r="J2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="U2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="U2" s="12"/>
       <c r="V2" s="0"/>
       <c r="W2" s="0"/>
       <c r="X2" s="0"/>
       <c r="Y2" s="0"/>
-      <c r="Z2" s="11"/>
+      <c r="Z2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="11"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="12"/>
       <c r="V3" s="0"/>
       <c r="W3" s="0"/>
       <c r="X3" s="0"/>
       <c r="Y3" s="0"/>
-      <c r="Z3" s="11"/>
+      <c r="Z3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14" t="s">
+      <c r="E4" s="14"/>
+      <c r="F4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="15" t="s">
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="16" t="s">
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16" t="s">
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16" t="s">
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16" t="s">
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="17" t="s">
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="AB4" s="17"/>
-      <c r="AC4" s="17"/>
+      <c r="AB4" s="18"/>
+      <c r="AC4" s="18"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="T5" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="V5" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB5" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC5" s="29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" s="30" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="31" t="n">
+        <v>25</v>
+      </c>
+      <c r="C6" s="31" t="n">
+        <v>10</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="O6" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="P6" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="N5" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="P5" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q5" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="R5" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="S5" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="T5" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U5" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="V5" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="W5" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="X5" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y5" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z5" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA5" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB5" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC5" s="28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" s="29" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="30" t="n">
-        <v>25</v>
-      </c>
-      <c r="C6" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="L6" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="M6" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="N6" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="O6" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="P6" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q6" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="R6" s="43"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="44" t="n">
+      <c r="Q6" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="R6" s="45"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="46" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="V6" s="45" t="n">
+      <c r="V6" s="47" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="W6" s="45" t="n">
+      <c r="W6" s="47" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="X6" s="45" t="n">
+      <c r="X6" s="47" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Y6" s="45" t="n">
+      <c r="Y6" s="47" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z6" s="46" t="n">
+      <c r="Z6" s="48" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="47"/>
-      <c r="AB6" s="42"/>
-      <c r="AC6" s="42"/>
+      <c r="AA6" s="49"/>
+      <c r="AB6" s="44"/>
+      <c r="AC6" s="44"/>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="48" t="n">
+      <c r="B7" s="50" t="n">
         <v>25</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="49" t="s">
+      <c r="C7" s="50"/>
+      <c r="D7" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="50"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="54"/>
-      <c r="T7" s="55"/>
-      <c r="U7" s="56"/>
-      <c r="V7" s="57"/>
-      <c r="W7" s="57"/>
-      <c r="X7" s="57"/>
-      <c r="Y7" s="57"/>
-      <c r="Z7" s="58"/>
-      <c r="AA7" s="59"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="56"/>
+      <c r="O7" s="55"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="56"/>
+      <c r="T7" s="57"/>
+      <c r="U7" s="58"/>
+      <c r="V7" s="59"/>
+      <c r="W7" s="59"/>
+      <c r="X7" s="59"/>
+      <c r="Y7" s="59"/>
+      <c r="Z7" s="60"/>
+      <c r="AA7" s="61"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="48" t="n">
+      <c r="B8" s="50" t="n">
         <v>100</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="49" t="s">
+      <c r="C8" s="50"/>
+      <c r="D8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="50"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="53"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="54"/>
-      <c r="T8" s="55"/>
-      <c r="U8" s="56"/>
-      <c r="V8" s="57"/>
-      <c r="W8" s="57"/>
-      <c r="X8" s="57"/>
-      <c r="Y8" s="57"/>
-      <c r="Z8" s="58"/>
-      <c r="AA8" s="59"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="55"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="56"/>
+      <c r="T8" s="57"/>
+      <c r="U8" s="58"/>
+      <c r="V8" s="59"/>
+      <c r="W8" s="59"/>
+      <c r="X8" s="59"/>
+      <c r="Y8" s="59"/>
+      <c r="Z8" s="60"/>
+      <c r="AA8" s="61"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="48" t="n">
+      <c r="B9" s="50" t="n">
         <v>150</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="49" t="s">
+      <c r="C9" s="50"/>
+      <c r="D9" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="53"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="54"/>
-      <c r="T9" s="55"/>
-      <c r="U9" s="56"/>
-      <c r="V9" s="57"/>
-      <c r="W9" s="57"/>
-      <c r="X9" s="57"/>
-      <c r="Y9" s="57"/>
-      <c r="Z9" s="58"/>
-      <c r="AA9" s="59"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="55"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="56"/>
+      <c r="T9" s="57"/>
+      <c r="U9" s="58"/>
+      <c r="V9" s="59"/>
+      <c r="W9" s="59"/>
+      <c r="X9" s="59"/>
+      <c r="Y9" s="59"/>
+      <c r="Z9" s="60"/>
+      <c r="AA9" s="61"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="48" t="n">
+      <c r="B10" s="50" t="n">
         <v>200</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49" t="s">
+      <c r="C10" s="50"/>
+      <c r="D10" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="53"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="54"/>
-      <c r="T10" s="55"/>
-      <c r="U10" s="56"/>
-      <c r="V10" s="57"/>
-      <c r="W10" s="57"/>
-      <c r="X10" s="57"/>
-      <c r="Y10" s="57"/>
-      <c r="Z10" s="58"/>
-      <c r="AA10" s="59"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="55"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="56"/>
+      <c r="T10" s="57"/>
+      <c r="U10" s="58"/>
+      <c r="V10" s="59"/>
+      <c r="W10" s="59"/>
+      <c r="X10" s="59"/>
+      <c r="Y10" s="59"/>
+      <c r="Z10" s="60"/>
+      <c r="AA10" s="61"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="48" t="n">
+      <c r="B11" s="50" t="n">
         <v>250</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="49" t="s">
+      <c r="C11" s="50"/>
+      <c r="D11" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="53"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="54"/>
-      <c r="T11" s="55"/>
-      <c r="U11" s="56"/>
-      <c r="V11" s="57"/>
-      <c r="W11" s="57"/>
-      <c r="X11" s="57"/>
-      <c r="Y11" s="57"/>
-      <c r="Z11" s="58"/>
-      <c r="AA11" s="59"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="55"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="56"/>
+      <c r="T11" s="57"/>
+      <c r="U11" s="58"/>
+      <c r="V11" s="59"/>
+      <c r="W11" s="59"/>
+      <c r="X11" s="59"/>
+      <c r="Y11" s="59"/>
+      <c r="Z11" s="60"/>
+      <c r="AA11" s="61"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="48" t="n">
+      <c r="B12" s="50" t="n">
         <v>300</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="49" t="s">
+      <c r="C12" s="50"/>
+      <c r="D12" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="54"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="54"/>
-      <c r="T12" s="55"/>
-      <c r="U12" s="56"/>
-      <c r="V12" s="57"/>
-      <c r="W12" s="57"/>
-      <c r="X12" s="57"/>
-      <c r="Y12" s="57"/>
-      <c r="Z12" s="58"/>
-      <c r="AA12" s="59"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="55"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="55"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="56"/>
+      <c r="T12" s="57"/>
+      <c r="U12" s="58"/>
+      <c r="V12" s="59"/>
+      <c r="W12" s="59"/>
+      <c r="X12" s="59"/>
+      <c r="Y12" s="59"/>
+      <c r="Z12" s="60"/>
+      <c r="AA12" s="61"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="48" t="n">
+      <c r="B13" s="50" t="n">
         <v>350</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="49" t="s">
+      <c r="C13" s="50"/>
+      <c r="D13" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="53"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="54"/>
-      <c r="O13" s="53"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="54"/>
-      <c r="T13" s="55"/>
-      <c r="U13" s="56"/>
-      <c r="V13" s="57"/>
-      <c r="W13" s="57"/>
-      <c r="X13" s="57"/>
-      <c r="Y13" s="57"/>
-      <c r="Z13" s="58"/>
-      <c r="AA13" s="59"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="55"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="55"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="56"/>
+      <c r="T13" s="57"/>
+      <c r="U13" s="58"/>
+      <c r="V13" s="59"/>
+      <c r="W13" s="59"/>
+      <c r="X13" s="59"/>
+      <c r="Y13" s="59"/>
+      <c r="Z13" s="60"/>
+      <c r="AA13" s="61"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="48" t="n">
+      <c r="B14" s="50" t="n">
         <v>400</v>
       </c>
-      <c r="C14" s="48"/>
-      <c r="D14" s="49" t="s">
+      <c r="C14" s="50"/>
+      <c r="D14" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="53"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="54"/>
-      <c r="T14" s="55"/>
-      <c r="U14" s="56"/>
-      <c r="V14" s="57"/>
-      <c r="W14" s="57"/>
-      <c r="X14" s="57"/>
-      <c r="Y14" s="57"/>
-      <c r="Z14" s="58"/>
-      <c r="AA14" s="59"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="55"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="56"/>
+      <c r="T14" s="57"/>
+      <c r="U14" s="58"/>
+      <c r="V14" s="59"/>
+      <c r="W14" s="59"/>
+      <c r="X14" s="59"/>
+      <c r="Y14" s="59"/>
+      <c r="Z14" s="60"/>
+      <c r="AA14" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -3036,7 +3078,7 @@
       <selection pane="bottomRight" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.78515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
@@ -3094,511 +3136,511 @@
         <v>Version: 8</v>
       </c>
       <c r="C2" s="5"/>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="7" t="s">
+      <c r="I2" s="7"/>
+      <c r="J2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="K2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-      <c r="U2" s="11"/>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
+      <c r="S2" s="11"/>
+      <c r="U2" s="12"/>
       <c r="V2" s="0"/>
       <c r="W2" s="0"/>
       <c r="X2" s="0"/>
       <c r="Y2" s="0"/>
-      <c r="Z2" s="11"/>
+      <c r="Z2" s="12"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="12"/>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-      <c r="L3" s="10"/>
-      <c r="N3" s="10"/>
-      <c r="O3" s="10"/>
-      <c r="Q3" s="10"/>
-      <c r="R3" s="10"/>
-      <c r="S3" s="10"/>
-      <c r="T3" s="10"/>
-      <c r="U3" s="11"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="12"/>
       <c r="V3" s="0"/>
       <c r="W3" s="0"/>
       <c r="X3" s="0"/>
       <c r="Y3" s="0"/>
-      <c r="Z3" s="11"/>
+      <c r="Z3" s="12"/>
     </row>
     <row r="4" customFormat="false" ht="23.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14" t="s">
+      <c r="E4" s="14"/>
+      <c r="F4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="15" t="s">
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="16" t="s">
+      <c r="J4" s="16"/>
+      <c r="K4" s="16"/>
+      <c r="L4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="16"/>
-      <c r="N4" s="16"/>
-      <c r="O4" s="16" t="s">
+      <c r="M4" s="17"/>
+      <c r="N4" s="17"/>
+      <c r="O4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="16"/>
-      <c r="Q4" s="16"/>
-      <c r="R4" s="16" t="s">
+      <c r="P4" s="17"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="S4" s="16"/>
-      <c r="T4" s="16"/>
-      <c r="U4" s="16" t="s">
+      <c r="S4" s="17"/>
+      <c r="T4" s="17"/>
+      <c r="U4" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="16"/>
-      <c r="W4" s="16"/>
-      <c r="X4" s="16"/>
-      <c r="Y4" s="16"/>
-      <c r="Z4" s="16"/>
-      <c r="AA4" s="17" t="s">
+      <c r="V4" s="17"/>
+      <c r="W4" s="17"/>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17"/>
+      <c r="Z4" s="17"/>
+      <c r="AA4" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="AB4" s="17"/>
-      <c r="AC4" s="17"/>
+      <c r="AB4" s="18"/>
+      <c r="AC4" s="18"/>
     </row>
     <row r="5" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="18" t="s">
+      <c r="B5" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" s="24" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="M5" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="N5" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="O5" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="P5" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q5" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="R5" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="S5" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="T5" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="V5" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="W5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="X5" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y5" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z5" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA5" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="AB5" s="29" t="s">
+        <v>42</v>
+      </c>
+      <c r="AC5" s="29" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" s="30" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="31" t="n">
+        <v>25</v>
+      </c>
+      <c r="C6" s="31" t="n">
+        <v>10</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="K6" s="38" t="s">
+        <v>50</v>
+      </c>
+      <c r="L6" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="M6" s="40" t="s">
+        <v>52</v>
+      </c>
+      <c r="N6" s="41" t="s">
+        <v>53</v>
+      </c>
+      <c r="O6" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="P6" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="C5" s="18" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="J5" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="K5" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="L5" s="24" t="s">
-        <v>25</v>
-      </c>
-      <c r="M5" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="N5" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="O5" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="P5" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q5" s="25" t="s">
-        <v>30</v>
-      </c>
-      <c r="R5" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="S5" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="T5" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="U5" s="19" t="s">
-        <v>34</v>
-      </c>
-      <c r="V5" s="18" t="s">
-        <v>35</v>
-      </c>
-      <c r="W5" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="X5" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y5" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="Z5" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA5" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB5" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC5" s="28" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" s="29" customFormat="true" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B6" s="30" t="n">
-        <v>25</v>
-      </c>
-      <c r="C6" s="30" t="n">
-        <v>10</v>
-      </c>
-      <c r="D6" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="30" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="H6" s="33" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="35" t="s">
-        <v>47</v>
-      </c>
-      <c r="K6" s="36" t="s">
-        <v>48</v>
-      </c>
-      <c r="L6" s="37" t="s">
-        <v>49</v>
-      </c>
-      <c r="M6" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="N6" s="39" t="s">
-        <v>51</v>
-      </c>
-      <c r="O6" s="40" t="s">
-        <v>52</v>
-      </c>
-      <c r="P6" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="Q6" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="R6" s="43"/>
-      <c r="S6" s="42"/>
-      <c r="T6" s="42"/>
-      <c r="U6" s="44" t="n">
+      <c r="Q6" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="R6" s="45"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="44"/>
+      <c r="U6" s="46" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="V6" s="45" t="n">
+      <c r="V6" s="47" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="W6" s="45" t="n">
+      <c r="W6" s="47" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="X6" s="45" t="n">
+      <c r="X6" s="47" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Y6" s="45" t="n">
+      <c r="Y6" s="47" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="Z6" s="46" t="n">
+      <c r="Z6" s="48" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA6" s="47"/>
-      <c r="AB6" s="42"/>
-      <c r="AC6" s="42"/>
+      <c r="AA6" s="49"/>
+      <c r="AB6" s="44"/>
+      <c r="AC6" s="44"/>
     </row>
     <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B7" s="48" t="n">
+      <c r="B7" s="50" t="n">
         <v>25</v>
       </c>
-      <c r="C7" s="48"/>
-      <c r="D7" s="49" t="s">
+      <c r="C7" s="50"/>
+      <c r="D7" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="50"/>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="51"/>
-      <c r="J7" s="52"/>
-      <c r="K7" s="48"/>
-      <c r="L7" s="53"/>
-      <c r="M7" s="50"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="53"/>
-      <c r="P7" s="29"/>
-      <c r="Q7" s="54"/>
-      <c r="T7" s="55"/>
-      <c r="U7" s="56"/>
-      <c r="V7" s="57"/>
-      <c r="W7" s="57"/>
-      <c r="X7" s="57"/>
-      <c r="Y7" s="57"/>
-      <c r="Z7" s="58"/>
-      <c r="AA7" s="59"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="13"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="54"/>
+      <c r="K7" s="50"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="52"/>
+      <c r="N7" s="56"/>
+      <c r="O7" s="55"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="56"/>
+      <c r="T7" s="57"/>
+      <c r="U7" s="58"/>
+      <c r="V7" s="59"/>
+      <c r="W7" s="59"/>
+      <c r="X7" s="59"/>
+      <c r="Y7" s="59"/>
+      <c r="Z7" s="60"/>
+      <c r="AA7" s="61"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B8" s="48" t="n">
+      <c r="B8" s="50" t="n">
         <v>100</v>
       </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="49" t="s">
+      <c r="C8" s="50"/>
+      <c r="D8" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="50"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-      <c r="H8" s="12"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="52"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="53"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="53"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="54"/>
-      <c r="T8" s="55"/>
-      <c r="U8" s="56"/>
-      <c r="V8" s="57"/>
-      <c r="W8" s="57"/>
-      <c r="X8" s="57"/>
-      <c r="Y8" s="57"/>
-      <c r="Z8" s="58"/>
-      <c r="AA8" s="59"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+      <c r="H8" s="13"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="54"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="55"/>
+      <c r="M8" s="52"/>
+      <c r="N8" s="56"/>
+      <c r="O8" s="55"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="56"/>
+      <c r="T8" s="57"/>
+      <c r="U8" s="58"/>
+      <c r="V8" s="59"/>
+      <c r="W8" s="59"/>
+      <c r="X8" s="59"/>
+      <c r="Y8" s="59"/>
+      <c r="Z8" s="60"/>
+      <c r="AA8" s="61"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B9" s="48" t="n">
+      <c r="B9" s="50" t="n">
         <v>150</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="49" t="s">
+      <c r="C9" s="50"/>
+      <c r="D9" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="29"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="12"/>
-      <c r="H9" s="12"/>
-      <c r="I9" s="51"/>
-      <c r="J9" s="52"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="53"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="53"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="54"/>
-      <c r="T9" s="55"/>
-      <c r="U9" s="56"/>
-      <c r="V9" s="57"/>
-      <c r="W9" s="57"/>
-      <c r="X9" s="57"/>
-      <c r="Y9" s="57"/>
-      <c r="Z9" s="58"/>
-      <c r="AA9" s="59"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="13"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13"/>
+      <c r="I9" s="53"/>
+      <c r="J9" s="54"/>
+      <c r="K9" s="50"/>
+      <c r="L9" s="55"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="56"/>
+      <c r="O9" s="55"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="56"/>
+      <c r="T9" s="57"/>
+      <c r="U9" s="58"/>
+      <c r="V9" s="59"/>
+      <c r="W9" s="59"/>
+      <c r="X9" s="59"/>
+      <c r="Y9" s="59"/>
+      <c r="Z9" s="60"/>
+      <c r="AA9" s="61"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="48" t="n">
+      <c r="B10" s="50" t="n">
         <v>200</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="49" t="s">
+      <c r="C10" s="50"/>
+      <c r="D10" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="51"/>
-      <c r="J10" s="52"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="50"/>
-      <c r="N10" s="54"/>
-      <c r="O10" s="53"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="54"/>
-      <c r="T10" s="55"/>
-      <c r="U10" s="56"/>
-      <c r="V10" s="57"/>
-      <c r="W10" s="57"/>
-      <c r="X10" s="57"/>
-      <c r="Y10" s="57"/>
-      <c r="Z10" s="58"/>
-      <c r="AA10" s="59"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="53"/>
+      <c r="J10" s="54"/>
+      <c r="K10" s="50"/>
+      <c r="L10" s="55"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="56"/>
+      <c r="O10" s="55"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="56"/>
+      <c r="T10" s="57"/>
+      <c r="U10" s="58"/>
+      <c r="V10" s="59"/>
+      <c r="W10" s="59"/>
+      <c r="X10" s="59"/>
+      <c r="Y10" s="59"/>
+      <c r="Z10" s="60"/>
+      <c r="AA10" s="61"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B11" s="48" t="n">
+      <c r="B11" s="50" t="n">
         <v>250</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="49" t="s">
+      <c r="C11" s="50"/>
+      <c r="D11" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="12"/>
-      <c r="I11" s="51"/>
-      <c r="J11" s="52"/>
-      <c r="K11" s="48"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="50"/>
-      <c r="N11" s="54"/>
-      <c r="O11" s="53"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="54"/>
-      <c r="T11" s="55"/>
-      <c r="U11" s="56"/>
-      <c r="V11" s="57"/>
-      <c r="W11" s="57"/>
-      <c r="X11" s="57"/>
-      <c r="Y11" s="57"/>
-      <c r="Z11" s="58"/>
-      <c r="AA11" s="59"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="50"/>
+      <c r="L11" s="55"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="56"/>
+      <c r="O11" s="55"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="56"/>
+      <c r="T11" s="57"/>
+      <c r="U11" s="58"/>
+      <c r="V11" s="59"/>
+      <c r="W11" s="59"/>
+      <c r="X11" s="59"/>
+      <c r="Y11" s="59"/>
+      <c r="Z11" s="60"/>
+      <c r="AA11" s="61"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B12" s="48" t="n">
+      <c r="B12" s="50" t="n">
         <v>300</v>
       </c>
-      <c r="C12" s="48"/>
-      <c r="D12" s="49" t="s">
+      <c r="C12" s="50"/>
+      <c r="D12" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="29"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="12"/>
-      <c r="I12" s="51"/>
-      <c r="J12" s="52"/>
-      <c r="K12" s="48"/>
-      <c r="L12" s="53"/>
-      <c r="M12" s="50"/>
-      <c r="N12" s="54"/>
-      <c r="O12" s="53"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="54"/>
-      <c r="T12" s="55"/>
-      <c r="U12" s="56"/>
-      <c r="V12" s="57"/>
-      <c r="W12" s="57"/>
-      <c r="X12" s="57"/>
-      <c r="Y12" s="57"/>
-      <c r="Z12" s="58"/>
-      <c r="AA12" s="59"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="54"/>
+      <c r="K12" s="50"/>
+      <c r="L12" s="55"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="56"/>
+      <c r="O12" s="55"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="56"/>
+      <c r="T12" s="57"/>
+      <c r="U12" s="58"/>
+      <c r="V12" s="59"/>
+      <c r="W12" s="59"/>
+      <c r="X12" s="59"/>
+      <c r="Y12" s="59"/>
+      <c r="Z12" s="60"/>
+      <c r="AA12" s="61"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B13" s="48" t="n">
+      <c r="B13" s="50" t="n">
         <v>350</v>
       </c>
-      <c r="C13" s="48"/>
-      <c r="D13" s="49" t="s">
+      <c r="C13" s="50"/>
+      <c r="D13" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E13" s="29"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="12"/>
-      <c r="I13" s="51"/>
-      <c r="J13" s="52"/>
-      <c r="K13" s="48"/>
-      <c r="L13" s="53"/>
-      <c r="M13" s="50"/>
-      <c r="N13" s="54"/>
-      <c r="O13" s="53"/>
-      <c r="P13" s="29"/>
-      <c r="Q13" s="54"/>
-      <c r="T13" s="55"/>
-      <c r="U13" s="56"/>
-      <c r="V13" s="57"/>
-      <c r="W13" s="57"/>
-      <c r="X13" s="57"/>
-      <c r="Y13" s="57"/>
-      <c r="Z13" s="58"/>
-      <c r="AA13" s="59"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13"/>
+      <c r="I13" s="53"/>
+      <c r="J13" s="54"/>
+      <c r="K13" s="50"/>
+      <c r="L13" s="55"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="56"/>
+      <c r="O13" s="55"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="56"/>
+      <c r="T13" s="57"/>
+      <c r="U13" s="58"/>
+      <c r="V13" s="59"/>
+      <c r="W13" s="59"/>
+      <c r="X13" s="59"/>
+      <c r="Y13" s="59"/>
+      <c r="Z13" s="60"/>
+      <c r="AA13" s="61"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B14" s="48" t="n">
+      <c r="B14" s="50" t="n">
         <v>400</v>
       </c>
-      <c r="C14" s="48"/>
-      <c r="D14" s="49" t="s">
+      <c r="C14" s="50"/>
+      <c r="D14" s="51" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="29"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="51"/>
-      <c r="J14" s="52"/>
-      <c r="K14" s="48"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="50"/>
-      <c r="N14" s="54"/>
-      <c r="O14" s="53"/>
-      <c r="P14" s="29"/>
-      <c r="Q14" s="54"/>
-      <c r="T14" s="55"/>
-      <c r="U14" s="56"/>
-      <c r="V14" s="57"/>
-      <c r="W14" s="57"/>
-      <c r="X14" s="57"/>
-      <c r="Y14" s="57"/>
-      <c r="Z14" s="58"/>
-      <c r="AA14" s="59"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="13"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="55"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="56"/>
+      <c r="O14" s="55"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="56"/>
+      <c r="T14" s="57"/>
+      <c r="U14" s="58"/>
+      <c r="V14" s="59"/>
+      <c r="W14" s="59"/>
+      <c r="X14" s="59"/>
+      <c r="Y14" s="59"/>
+      <c r="Z14" s="60"/>
+      <c r="AA14" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -3693,36 +3735,36 @@
       <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
   </cols>
   <sheetData>
-    <row r="1" s="60" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" s="60" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="28" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="3" s="60" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="28" t="n">
+    <row r="1" s="62" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="29" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" s="62" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" s="62" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="29" t="n">
         <v>8</v>
       </c>
     </row>
-    <row r="4" s="60" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="28"/>
-    </row>
-    <row r="5" s="60" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="60" t="s">
-        <v>58</v>
+    <row r="4" s="62" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="29"/>
+    </row>
+    <row r="5" s="62" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="62" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3730,7 +3772,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3738,7 +3780,7 @@
         <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3746,7 +3788,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3754,7 +3796,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3762,7 +3804,7 @@
         <v>5</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3770,7 +3812,7 @@
         <v>6</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3778,7 +3820,7 @@
         <v>7</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3786,7 +3828,7 @@
         <v>8</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update validity in plotting mode column in spreadsheets
remove redundant choices, add pilatus
</commit_message>
<xml_diff>
--- a/startup/xlsx/lakeshore.xlsx
+++ b/startup/xlsx/lakeshore.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="lakeshore1" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>BR</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -133,7 +133,7 @@
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>BR</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -252,7 +252,7 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>BR</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -371,7 +371,7 @@
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>BR</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -490,7 +490,7 @@
 <file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>BR</author>
+    <author> </author>
   </authors>
   <commentList>
     <comment ref="B1" authorId="0">
@@ -607,7 +607,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="77">
   <si>
     <t xml:space="preserve">LakeShore</t>
   </si>
@@ -835,6 +835,9 @@
   </si>
   <si>
     <t xml:space="preserve">remove experimenters cell, 5 tabs in template</t>
+  </si>
+  <si>
+    <t xml:space="preserve">update validity for plotting mode columns</t>
   </si>
 </sst>
 </file>
@@ -1186,7 +1189,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="69">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1405,6 +1408,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1542,9 +1549,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1625760</xdr:colOff>
+      <xdr:colOff>1625400</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>30600</xdr:rowOff>
+      <xdr:rowOff>30240</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1554,7 +1561,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5185800" y="6296400"/>
-          <a:ext cx="6653880" cy="1784880"/>
+          <a:ext cx="6654600" cy="1784160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1576,7 +1583,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -1787,9 +1794,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1356120</xdr:colOff>
+      <xdr:colOff>1355760</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>106560</xdr:rowOff>
+      <xdr:rowOff>106200</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1798,8 +1805,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4789080" y="7347600"/>
-          <a:ext cx="6653880" cy="1784880"/>
+          <a:off x="4789080" y="7347240"/>
+          <a:ext cx="6654600" cy="1784520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1821,7 +1828,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -2032,9 +2039,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>824760</xdr:colOff>
+      <xdr:colOff>824400</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>30960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2044,7 +2051,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4316400" y="7434720"/>
-          <a:ext cx="6653880" cy="1784880"/>
+          <a:ext cx="6654600" cy="1784520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2066,7 +2073,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -2277,9 +2284,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>853920</xdr:colOff>
+      <xdr:colOff>853560</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>30960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2289,7 +2296,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4316400" y="7434720"/>
-          <a:ext cx="6653880" cy="1784880"/>
+          <a:ext cx="6653160" cy="1784520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2311,7 +2318,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -2522,9 +2529,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>775440</xdr:colOff>
+      <xdr:colOff>775080</xdr:colOff>
       <xdr:row>50</xdr:row>
-      <xdr:rowOff>31320</xdr:rowOff>
+      <xdr:rowOff>30960</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -2534,7 +2541,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="4316400" y="7434720"/>
-          <a:ext cx="6653880" cy="1784880"/>
+          <a:ext cx="6654600" cy="1784520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2556,7 +2563,7 @@
         <a:fontRef idx="minor"/>
       </xdr:style>
       <xdr:txBody>
-        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360" anchor="t">
+        <a:bodyPr lIns="73080" rIns="36360" tIns="36360" bIns="36360">
           <a:noAutofit/>
         </a:bodyPr>
         <a:p>
@@ -2763,15 +2770,15 @@
   </sheetPr>
   <dimension ref="B1:AF14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="6" ySplit="6" topLeftCell="G7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="L6" activeCellId="0" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
@@ -2829,7 +2836,7 @@
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 14</v>
+        <v>Version: 15</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -3130,24 +3137,24 @@
       <c r="F7" s="54"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="56"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="57"/>
       <c r="L7" s="52"/>
-      <c r="M7" s="57"/>
+      <c r="M7" s="58"/>
       <c r="N7" s="54"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="57"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="58"/>
       <c r="Q7" s="31"/>
-      <c r="R7" s="58"/>
-      <c r="W7" s="59"/>
-      <c r="X7" s="60"/>
-      <c r="Y7" s="61"/>
-      <c r="Z7" s="61"/>
-      <c r="AA7" s="61"/>
-      <c r="AB7" s="61"/>
-      <c r="AC7" s="62"/>
-      <c r="AD7" s="63"/>
+      <c r="R7" s="59"/>
+      <c r="W7" s="60"/>
+      <c r="X7" s="61"/>
+      <c r="Y7" s="62"/>
+      <c r="Z7" s="62"/>
+      <c r="AA7" s="62"/>
+      <c r="AB7" s="62"/>
+      <c r="AC7" s="63"/>
+      <c r="AD7" s="64"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="52" t="n">
@@ -3161,24 +3168,24 @@
       <c r="F8" s="54"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="56"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="57"/>
       <c r="L8" s="52"/>
-      <c r="M8" s="57"/>
+      <c r="M8" s="58"/>
       <c r="N8" s="54"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="57"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="58"/>
       <c r="Q8" s="31"/>
-      <c r="R8" s="58"/>
-      <c r="W8" s="59"/>
-      <c r="X8" s="60"/>
-      <c r="Y8" s="61"/>
-      <c r="Z8" s="61"/>
-      <c r="AA8" s="61"/>
-      <c r="AB8" s="61"/>
-      <c r="AC8" s="62"/>
-      <c r="AD8" s="63"/>
+      <c r="R8" s="59"/>
+      <c r="W8" s="60"/>
+      <c r="X8" s="61"/>
+      <c r="Y8" s="62"/>
+      <c r="Z8" s="62"/>
+      <c r="AA8" s="62"/>
+      <c r="AB8" s="62"/>
+      <c r="AC8" s="63"/>
+      <c r="AD8" s="64"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="52" t="n">
@@ -3192,24 +3199,24 @@
       <c r="F9" s="31"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="56"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="57"/>
       <c r="L9" s="52"/>
-      <c r="M9" s="57"/>
+      <c r="M9" s="58"/>
       <c r="N9" s="54"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="57"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="58"/>
       <c r="Q9" s="31"/>
-      <c r="R9" s="58"/>
-      <c r="W9" s="59"/>
-      <c r="X9" s="60"/>
-      <c r="Y9" s="61"/>
-      <c r="Z9" s="61"/>
-      <c r="AA9" s="61"/>
-      <c r="AB9" s="61"/>
-      <c r="AC9" s="62"/>
-      <c r="AD9" s="63"/>
+      <c r="R9" s="59"/>
+      <c r="W9" s="60"/>
+      <c r="X9" s="61"/>
+      <c r="Y9" s="62"/>
+      <c r="Z9" s="62"/>
+      <c r="AA9" s="62"/>
+      <c r="AB9" s="62"/>
+      <c r="AC9" s="63"/>
+      <c r="AD9" s="64"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="52" t="n">
@@ -3223,24 +3230,24 @@
       <c r="F10" s="31"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="56"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="57"/>
       <c r="L10" s="52"/>
-      <c r="M10" s="57"/>
+      <c r="M10" s="58"/>
       <c r="N10" s="54"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="57"/>
+      <c r="O10" s="59"/>
+      <c r="P10" s="58"/>
       <c r="Q10" s="31"/>
-      <c r="R10" s="58"/>
-      <c r="W10" s="59"/>
-      <c r="X10" s="60"/>
-      <c r="Y10" s="61"/>
-      <c r="Z10" s="61"/>
-      <c r="AA10" s="61"/>
-      <c r="AB10" s="61"/>
-      <c r="AC10" s="62"/>
-      <c r="AD10" s="63"/>
+      <c r="R10" s="59"/>
+      <c r="W10" s="60"/>
+      <c r="X10" s="61"/>
+      <c r="Y10" s="62"/>
+      <c r="Z10" s="62"/>
+      <c r="AA10" s="62"/>
+      <c r="AB10" s="62"/>
+      <c r="AC10" s="63"/>
+      <c r="AD10" s="64"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="52" t="n">
@@ -3254,24 +3261,24 @@
       <c r="F11" s="31"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="57"/>
       <c r="L11" s="52"/>
-      <c r="M11" s="57"/>
+      <c r="M11" s="58"/>
       <c r="N11" s="54"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="57"/>
+      <c r="O11" s="59"/>
+      <c r="P11" s="58"/>
       <c r="Q11" s="31"/>
-      <c r="R11" s="58"/>
-      <c r="W11" s="59"/>
-      <c r="X11" s="60"/>
-      <c r="Y11" s="61"/>
-      <c r="Z11" s="61"/>
-      <c r="AA11" s="61"/>
-      <c r="AB11" s="61"/>
-      <c r="AC11" s="62"/>
-      <c r="AD11" s="63"/>
+      <c r="R11" s="59"/>
+      <c r="W11" s="60"/>
+      <c r="X11" s="61"/>
+      <c r="Y11" s="62"/>
+      <c r="Z11" s="62"/>
+      <c r="AA11" s="62"/>
+      <c r="AB11" s="62"/>
+      <c r="AC11" s="63"/>
+      <c r="AD11" s="64"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="52" t="n">
@@ -3285,24 +3292,24 @@
       <c r="F12" s="31"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="56"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="57"/>
       <c r="L12" s="52"/>
-      <c r="M12" s="57"/>
+      <c r="M12" s="58"/>
       <c r="N12" s="54"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="57"/>
+      <c r="O12" s="59"/>
+      <c r="P12" s="58"/>
       <c r="Q12" s="31"/>
-      <c r="R12" s="58"/>
-      <c r="W12" s="59"/>
-      <c r="X12" s="60"/>
-      <c r="Y12" s="61"/>
-      <c r="Z12" s="61"/>
-      <c r="AA12" s="61"/>
-      <c r="AB12" s="61"/>
-      <c r="AC12" s="62"/>
-      <c r="AD12" s="63"/>
+      <c r="R12" s="59"/>
+      <c r="W12" s="60"/>
+      <c r="X12" s="61"/>
+      <c r="Y12" s="62"/>
+      <c r="Z12" s="62"/>
+      <c r="AA12" s="62"/>
+      <c r="AB12" s="62"/>
+      <c r="AC12" s="63"/>
+      <c r="AD12" s="64"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="52"/>
@@ -3313,23 +3320,23 @@
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="56"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="52"/>
-      <c r="M13" s="57"/>
+      <c r="M13" s="58"/>
       <c r="N13" s="54"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="57"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="58"/>
       <c r="Q13" s="31"/>
-      <c r="R13" s="58"/>
-      <c r="W13" s="59"/>
-      <c r="X13" s="60"/>
-      <c r="Y13" s="61"/>
-      <c r="Z13" s="61"/>
-      <c r="AA13" s="61"/>
-      <c r="AB13" s="61"/>
-      <c r="AC13" s="62"/>
-      <c r="AD13" s="63"/>
+      <c r="R13" s="59"/>
+      <c r="W13" s="60"/>
+      <c r="X13" s="61"/>
+      <c r="Y13" s="62"/>
+      <c r="Z13" s="62"/>
+      <c r="AA13" s="62"/>
+      <c r="AB13" s="62"/>
+      <c r="AC13" s="63"/>
+      <c r="AD13" s="64"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="52"/>
@@ -3340,23 +3347,23 @@
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
       <c r="I14" s="14"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="56"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="57"/>
       <c r="L14" s="52"/>
-      <c r="M14" s="57"/>
+      <c r="M14" s="58"/>
       <c r="N14" s="54"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="57"/>
+      <c r="O14" s="59"/>
+      <c r="P14" s="58"/>
       <c r="Q14" s="31"/>
-      <c r="R14" s="58"/>
-      <c r="W14" s="59"/>
-      <c r="X14" s="60"/>
-      <c r="Y14" s="61"/>
-      <c r="Z14" s="61"/>
-      <c r="AA14" s="61"/>
-      <c r="AB14" s="61"/>
-      <c r="AC14" s="62"/>
-      <c r="AD14" s="63"/>
+      <c r="R14" s="59"/>
+      <c r="W14" s="60"/>
+      <c r="X14" s="61"/>
+      <c r="Y14" s="62"/>
+      <c r="Z14" s="62"/>
+      <c r="AA14" s="62"/>
+      <c r="AB14" s="62"/>
+      <c r="AC14" s="63"/>
+      <c r="AD14" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -3373,78 +3380,78 @@
     <mergeCell ref="AD4:AF4"/>
   </mergeCells>
   <dataValidations count="17">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:C12 B13:D70" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:C12 B13:D70" type="decimal">
       <formula1>-277</formula1>
       <formula2>500</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D6:D12" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D6:D12" type="list">
       <formula1>"low,medium,high"</formula1>
       <formula2>500</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X6:AC14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 E6:E14" type="list">
+      <formula1>"Yes,No"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+      <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end,Temperature at beginning,Temperature at end,Temperature+element at beginning,Temperature+element at end,Temperature+element+edge at beginning,Temperature+element+edge at "</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
+      <formula1>1</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X6:AC14" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AD6:AF6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AD6:AF6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6:L14" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G14" type="whole">
+      <formula1>0</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I13:I14" type="list">
+      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J14" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:W6" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W7:W14" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6:L14" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G14" type="whole">
-      <formula1>0</formula1>
-      <formula2>1000</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
-      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I12" type="list">
+      <formula1>"transmission,fluorescence,reference,yield,pilatus,test,"</formula1>
       <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I14" type="list">
-      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J14" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:W6" type="none">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 E6:E14" type="list">
-      <formula1>"Yes,No"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
-      <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end,Temperature at beginning,Temperature at end,Temperature+element at beginning,Temperature+element at end,Temperature+element+edge at beginning,Temperature+element+edge at "</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
-      <formula1>1</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W7:W14" type="none">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3466,10 +3473,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="L6" activeCellId="0" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
@@ -3496,10 +3503,10 @@
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="64"/>
+      <c r="E1" s="65"/>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
@@ -3528,7 +3535,7 @@
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 14</v>
+        <v>Version: 15</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -3542,7 +3549,7 @@
       <c r="K2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="65" t="s">
+      <c r="L2" s="66" t="s">
         <v>5</v>
       </c>
       <c r="M2" s="8" t="s">
@@ -3828,24 +3835,24 @@
       <c r="F7" s="54"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="56"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="57"/>
       <c r="L7" s="52"/>
-      <c r="M7" s="57"/>
+      <c r="M7" s="58"/>
       <c r="N7" s="54"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="57"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="58"/>
       <c r="Q7" s="31"/>
-      <c r="R7" s="58"/>
-      <c r="W7" s="59"/>
-      <c r="X7" s="60"/>
-      <c r="Y7" s="61"/>
-      <c r="Z7" s="61"/>
-      <c r="AA7" s="61"/>
-      <c r="AB7" s="61"/>
-      <c r="AC7" s="62"/>
-      <c r="AD7" s="63"/>
+      <c r="R7" s="59"/>
+      <c r="W7" s="60"/>
+      <c r="X7" s="61"/>
+      <c r="Y7" s="62"/>
+      <c r="Z7" s="62"/>
+      <c r="AA7" s="62"/>
+      <c r="AB7" s="62"/>
+      <c r="AC7" s="63"/>
+      <c r="AD7" s="64"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="52" t="n">
@@ -3859,24 +3866,24 @@
       <c r="F8" s="54"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="56"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="57"/>
       <c r="L8" s="52"/>
-      <c r="M8" s="57"/>
+      <c r="M8" s="58"/>
       <c r="N8" s="54"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="57"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="58"/>
       <c r="Q8" s="31"/>
-      <c r="R8" s="58"/>
-      <c r="W8" s="59"/>
-      <c r="X8" s="60"/>
-      <c r="Y8" s="61"/>
-      <c r="Z8" s="61"/>
-      <c r="AA8" s="61"/>
-      <c r="AB8" s="61"/>
-      <c r="AC8" s="62"/>
-      <c r="AD8" s="63"/>
+      <c r="R8" s="59"/>
+      <c r="W8" s="60"/>
+      <c r="X8" s="61"/>
+      <c r="Y8" s="62"/>
+      <c r="Z8" s="62"/>
+      <c r="AA8" s="62"/>
+      <c r="AB8" s="62"/>
+      <c r="AC8" s="63"/>
+      <c r="AD8" s="64"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="52" t="n">
@@ -3890,24 +3897,24 @@
       <c r="F9" s="31"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="56"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="57"/>
       <c r="L9" s="52"/>
-      <c r="M9" s="57"/>
+      <c r="M9" s="58"/>
       <c r="N9" s="54"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="57"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="58"/>
       <c r="Q9" s="31"/>
-      <c r="R9" s="58"/>
-      <c r="W9" s="59"/>
-      <c r="X9" s="60"/>
-      <c r="Y9" s="61"/>
-      <c r="Z9" s="61"/>
-      <c r="AA9" s="61"/>
-      <c r="AB9" s="61"/>
-      <c r="AC9" s="62"/>
-      <c r="AD9" s="63"/>
+      <c r="R9" s="59"/>
+      <c r="W9" s="60"/>
+      <c r="X9" s="61"/>
+      <c r="Y9" s="62"/>
+      <c r="Z9" s="62"/>
+      <c r="AA9" s="62"/>
+      <c r="AB9" s="62"/>
+      <c r="AC9" s="63"/>
+      <c r="AD9" s="64"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="52" t="n">
@@ -3921,24 +3928,24 @@
       <c r="F10" s="31"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="56"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="57"/>
       <c r="L10" s="52"/>
-      <c r="M10" s="57"/>
+      <c r="M10" s="58"/>
       <c r="N10" s="54"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="57"/>
+      <c r="O10" s="59"/>
+      <c r="P10" s="58"/>
       <c r="Q10" s="31"/>
-      <c r="R10" s="58"/>
-      <c r="W10" s="59"/>
-      <c r="X10" s="60"/>
-      <c r="Y10" s="61"/>
-      <c r="Z10" s="61"/>
-      <c r="AA10" s="61"/>
-      <c r="AB10" s="61"/>
-      <c r="AC10" s="62"/>
-      <c r="AD10" s="63"/>
+      <c r="R10" s="59"/>
+      <c r="W10" s="60"/>
+      <c r="X10" s="61"/>
+      <c r="Y10" s="62"/>
+      <c r="Z10" s="62"/>
+      <c r="AA10" s="62"/>
+      <c r="AB10" s="62"/>
+      <c r="AC10" s="63"/>
+      <c r="AD10" s="64"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="52" t="n">
@@ -3952,24 +3959,24 @@
       <c r="F11" s="31"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="57"/>
       <c r="L11" s="52"/>
-      <c r="M11" s="57"/>
+      <c r="M11" s="58"/>
       <c r="N11" s="54"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="57"/>
+      <c r="O11" s="59"/>
+      <c r="P11" s="58"/>
       <c r="Q11" s="31"/>
-      <c r="R11" s="58"/>
-      <c r="W11" s="59"/>
-      <c r="X11" s="60"/>
-      <c r="Y11" s="61"/>
-      <c r="Z11" s="61"/>
-      <c r="AA11" s="61"/>
-      <c r="AB11" s="61"/>
-      <c r="AC11" s="62"/>
-      <c r="AD11" s="63"/>
+      <c r="R11" s="59"/>
+      <c r="W11" s="60"/>
+      <c r="X11" s="61"/>
+      <c r="Y11" s="62"/>
+      <c r="Z11" s="62"/>
+      <c r="AA11" s="62"/>
+      <c r="AB11" s="62"/>
+      <c r="AC11" s="63"/>
+      <c r="AD11" s="64"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="52" t="n">
@@ -3983,24 +3990,24 @@
       <c r="F12" s="31"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="56"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="57"/>
       <c r="L12" s="52"/>
-      <c r="M12" s="57"/>
+      <c r="M12" s="58"/>
       <c r="N12" s="54"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="57"/>
+      <c r="O12" s="59"/>
+      <c r="P12" s="58"/>
       <c r="Q12" s="31"/>
-      <c r="R12" s="58"/>
-      <c r="W12" s="59"/>
-      <c r="X12" s="60"/>
-      <c r="Y12" s="61"/>
-      <c r="Z12" s="61"/>
-      <c r="AA12" s="61"/>
-      <c r="AB12" s="61"/>
-      <c r="AC12" s="62"/>
-      <c r="AD12" s="63"/>
+      <c r="R12" s="59"/>
+      <c r="W12" s="60"/>
+      <c r="X12" s="61"/>
+      <c r="Y12" s="62"/>
+      <c r="Z12" s="62"/>
+      <c r="AA12" s="62"/>
+      <c r="AB12" s="62"/>
+      <c r="AC12" s="63"/>
+      <c r="AD12" s="64"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="52" t="n">
@@ -4014,24 +4021,24 @@
       <c r="F13" s="31"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="56"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="52"/>
-      <c r="M13" s="57"/>
+      <c r="M13" s="58"/>
       <c r="N13" s="54"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="57"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="58"/>
       <c r="Q13" s="31"/>
-      <c r="R13" s="58"/>
-      <c r="W13" s="59"/>
-      <c r="X13" s="60"/>
-      <c r="Y13" s="61"/>
-      <c r="Z13" s="61"/>
-      <c r="AA13" s="61"/>
-      <c r="AB13" s="61"/>
-      <c r="AC13" s="62"/>
-      <c r="AD13" s="63"/>
+      <c r="R13" s="59"/>
+      <c r="W13" s="60"/>
+      <c r="X13" s="61"/>
+      <c r="Y13" s="62"/>
+      <c r="Z13" s="62"/>
+      <c r="AA13" s="62"/>
+      <c r="AB13" s="62"/>
+      <c r="AC13" s="63"/>
+      <c r="AD13" s="64"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="52" t="n">
@@ -4045,24 +4052,24 @@
       <c r="F14" s="31"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="56"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="57"/>
       <c r="L14" s="52"/>
-      <c r="M14" s="57"/>
+      <c r="M14" s="58"/>
       <c r="N14" s="54"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="57"/>
+      <c r="O14" s="59"/>
+      <c r="P14" s="58"/>
       <c r="Q14" s="31"/>
-      <c r="R14" s="58"/>
-      <c r="W14" s="59"/>
-      <c r="X14" s="60"/>
-      <c r="Y14" s="61"/>
-      <c r="Z14" s="61"/>
-      <c r="AA14" s="61"/>
-      <c r="AB14" s="61"/>
-      <c r="AC14" s="62"/>
-      <c r="AD14" s="63"/>
+      <c r="R14" s="59"/>
+      <c r="W14" s="60"/>
+      <c r="X14" s="61"/>
+      <c r="Y14" s="62"/>
+      <c r="Z14" s="62"/>
+      <c r="AA14" s="62"/>
+      <c r="AB14" s="62"/>
+      <c r="AC14" s="63"/>
+      <c r="AD14" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -4078,87 +4085,83 @@
     <mergeCell ref="X4:AC4"/>
     <mergeCell ref="AD4:AF4"/>
   </mergeCells>
-  <dataValidations count="19">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:C12 B13:D70" type="decimal">
+  <dataValidations count="18">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:C12 B13:D70" type="decimal">
       <formula1>-277</formula1>
       <formula2>500</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D6 D8:D12" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D6 D8:D12" type="list">
       <formula1>"low,medium,high"</formula1>
       <formula2>500</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 E6:E14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 E6:E14" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end,Temperature at beginning,Temperature at end,Temperature+element at beginning,Temperature+element at end,Temperature+element+edge at beginning,Temperature+element+edge at "</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X6:AC6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X6:AC6" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AD6:AF6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AD6:AF6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X7:AC14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X7:AC14" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L7:L14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L7:L14" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G14" type="whole">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G14" type="whole">
       <formula1>0</formula1>
       <formula2>1000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
-      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I14" type="list">
-      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J14" type="list">
       <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:W6" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:W6" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W7:W14" type="none">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="W7:W14" type="none">
       <formula1>10</formula1>
       <formula2>210</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6" type="list">
       <formula1>"unfocused,focused"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I14" type="list">
+      <formula1>"transmission,fluorescence,reference,yield,pilatus,test,"</formula1>
       <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4180,10 +4183,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="L6" activeCellId="0" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
@@ -4209,7 +4212,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="65" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="4"/>
@@ -4240,7 +4243,7 @@
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 14</v>
+        <v>Version: 15</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -4254,7 +4257,7 @@
       <c r="K2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="65" t="s">
+      <c r="L2" s="66" t="s">
         <v>5</v>
       </c>
       <c r="M2" s="8" t="s">
@@ -4540,24 +4543,24 @@
       <c r="F7" s="54"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="56"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="57"/>
       <c r="L7" s="52"/>
-      <c r="M7" s="57"/>
+      <c r="M7" s="58"/>
       <c r="N7" s="54"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="57"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="58"/>
       <c r="Q7" s="31"/>
-      <c r="R7" s="58"/>
-      <c r="W7" s="59"/>
-      <c r="X7" s="60"/>
-      <c r="Y7" s="61"/>
-      <c r="Z7" s="61"/>
-      <c r="AA7" s="61"/>
-      <c r="AB7" s="61"/>
-      <c r="AC7" s="62"/>
-      <c r="AD7" s="63"/>
+      <c r="R7" s="59"/>
+      <c r="W7" s="60"/>
+      <c r="X7" s="61"/>
+      <c r="Y7" s="62"/>
+      <c r="Z7" s="62"/>
+      <c r="AA7" s="62"/>
+      <c r="AB7" s="62"/>
+      <c r="AC7" s="63"/>
+      <c r="AD7" s="64"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="52" t="n">
@@ -4571,24 +4574,24 @@
       <c r="F8" s="54"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="56"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="57"/>
       <c r="L8" s="52"/>
-      <c r="M8" s="57"/>
+      <c r="M8" s="58"/>
       <c r="N8" s="54"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="57"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="58"/>
       <c r="Q8" s="31"/>
-      <c r="R8" s="58"/>
-      <c r="W8" s="59"/>
-      <c r="X8" s="60"/>
-      <c r="Y8" s="61"/>
-      <c r="Z8" s="61"/>
-      <c r="AA8" s="61"/>
-      <c r="AB8" s="61"/>
-      <c r="AC8" s="62"/>
-      <c r="AD8" s="63"/>
+      <c r="R8" s="59"/>
+      <c r="W8" s="60"/>
+      <c r="X8" s="61"/>
+      <c r="Y8" s="62"/>
+      <c r="Z8" s="62"/>
+      <c r="AA8" s="62"/>
+      <c r="AB8" s="62"/>
+      <c r="AC8" s="63"/>
+      <c r="AD8" s="64"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="52" t="n">
@@ -4602,24 +4605,24 @@
       <c r="F9" s="31"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="56"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="57"/>
       <c r="L9" s="52"/>
-      <c r="M9" s="57"/>
+      <c r="M9" s="58"/>
       <c r="N9" s="54"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="57"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="58"/>
       <c r="Q9" s="31"/>
-      <c r="R9" s="58"/>
-      <c r="W9" s="59"/>
-      <c r="X9" s="60"/>
-      <c r="Y9" s="61"/>
-      <c r="Z9" s="61"/>
-      <c r="AA9" s="61"/>
-      <c r="AB9" s="61"/>
-      <c r="AC9" s="62"/>
-      <c r="AD9" s="63"/>
+      <c r="R9" s="59"/>
+      <c r="W9" s="60"/>
+      <c r="X9" s="61"/>
+      <c r="Y9" s="62"/>
+      <c r="Z9" s="62"/>
+      <c r="AA9" s="62"/>
+      <c r="AB9" s="62"/>
+      <c r="AC9" s="63"/>
+      <c r="AD9" s="64"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="52" t="n">
@@ -4633,24 +4636,24 @@
       <c r="F10" s="31"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="56"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="57"/>
       <c r="L10" s="52"/>
-      <c r="M10" s="57"/>
+      <c r="M10" s="58"/>
       <c r="N10" s="54"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="57"/>
+      <c r="O10" s="59"/>
+      <c r="P10" s="58"/>
       <c r="Q10" s="31"/>
-      <c r="R10" s="58"/>
-      <c r="W10" s="59"/>
-      <c r="X10" s="60"/>
-      <c r="Y10" s="61"/>
-      <c r="Z10" s="61"/>
-      <c r="AA10" s="61"/>
-      <c r="AB10" s="61"/>
-      <c r="AC10" s="62"/>
-      <c r="AD10" s="63"/>
+      <c r="R10" s="59"/>
+      <c r="W10" s="60"/>
+      <c r="X10" s="61"/>
+      <c r="Y10" s="62"/>
+      <c r="Z10" s="62"/>
+      <c r="AA10" s="62"/>
+      <c r="AB10" s="62"/>
+      <c r="AC10" s="63"/>
+      <c r="AD10" s="64"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="52" t="n">
@@ -4664,24 +4667,24 @@
       <c r="F11" s="31"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="57"/>
       <c r="L11" s="52"/>
-      <c r="M11" s="57"/>
+      <c r="M11" s="58"/>
       <c r="N11" s="54"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="57"/>
+      <c r="O11" s="59"/>
+      <c r="P11" s="58"/>
       <c r="Q11" s="31"/>
-      <c r="R11" s="58"/>
-      <c r="W11" s="59"/>
-      <c r="X11" s="60"/>
-      <c r="Y11" s="61"/>
-      <c r="Z11" s="61"/>
-      <c r="AA11" s="61"/>
-      <c r="AB11" s="61"/>
-      <c r="AC11" s="62"/>
-      <c r="AD11" s="63"/>
+      <c r="R11" s="59"/>
+      <c r="W11" s="60"/>
+      <c r="X11" s="61"/>
+      <c r="Y11" s="62"/>
+      <c r="Z11" s="62"/>
+      <c r="AA11" s="62"/>
+      <c r="AB11" s="62"/>
+      <c r="AC11" s="63"/>
+      <c r="AD11" s="64"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="52" t="n">
@@ -4695,24 +4698,24 @@
       <c r="F12" s="31"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="56"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="57"/>
       <c r="L12" s="52"/>
-      <c r="M12" s="57"/>
+      <c r="M12" s="58"/>
       <c r="N12" s="54"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="57"/>
+      <c r="O12" s="59"/>
+      <c r="P12" s="58"/>
       <c r="Q12" s="31"/>
-      <c r="R12" s="58"/>
-      <c r="W12" s="59"/>
-      <c r="X12" s="60"/>
-      <c r="Y12" s="61"/>
-      <c r="Z12" s="61"/>
-      <c r="AA12" s="61"/>
-      <c r="AB12" s="61"/>
-      <c r="AC12" s="62"/>
-      <c r="AD12" s="63"/>
+      <c r="R12" s="59"/>
+      <c r="W12" s="60"/>
+      <c r="X12" s="61"/>
+      <c r="Y12" s="62"/>
+      <c r="Z12" s="62"/>
+      <c r="AA12" s="62"/>
+      <c r="AB12" s="62"/>
+      <c r="AC12" s="63"/>
+      <c r="AD12" s="64"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="52" t="n">
@@ -4726,24 +4729,24 @@
       <c r="F13" s="31"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="56"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="52"/>
-      <c r="M13" s="57"/>
+      <c r="M13" s="58"/>
       <c r="N13" s="54"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="57"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="58"/>
       <c r="Q13" s="31"/>
-      <c r="R13" s="58"/>
-      <c r="W13" s="59"/>
-      <c r="X13" s="60"/>
-      <c r="Y13" s="61"/>
-      <c r="Z13" s="61"/>
-      <c r="AA13" s="61"/>
-      <c r="AB13" s="61"/>
-      <c r="AC13" s="62"/>
-      <c r="AD13" s="63"/>
+      <c r="R13" s="59"/>
+      <c r="W13" s="60"/>
+      <c r="X13" s="61"/>
+      <c r="Y13" s="62"/>
+      <c r="Z13" s="62"/>
+      <c r="AA13" s="62"/>
+      <c r="AB13" s="62"/>
+      <c r="AC13" s="63"/>
+      <c r="AD13" s="64"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="52" t="n">
@@ -4757,24 +4760,24 @@
       <c r="F14" s="31"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="56"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="57"/>
       <c r="L14" s="52"/>
-      <c r="M14" s="57"/>
+      <c r="M14" s="58"/>
       <c r="N14" s="54"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="57"/>
+      <c r="O14" s="59"/>
+      <c r="P14" s="58"/>
       <c r="Q14" s="31"/>
-      <c r="R14" s="58"/>
-      <c r="W14" s="59"/>
-      <c r="X14" s="60"/>
-      <c r="Y14" s="61"/>
-      <c r="Z14" s="61"/>
-      <c r="AA14" s="61"/>
-      <c r="AB14" s="61"/>
-      <c r="AC14" s="62"/>
-      <c r="AD14" s="63"/>
+      <c r="R14" s="59"/>
+      <c r="W14" s="60"/>
+      <c r="X14" s="61"/>
+      <c r="Y14" s="62"/>
+      <c r="Z14" s="62"/>
+      <c r="AA14" s="62"/>
+      <c r="AB14" s="62"/>
+      <c r="AC14" s="63"/>
+      <c r="AD14" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -4790,79 +4793,75 @@
     <mergeCell ref="X4:AC4"/>
     <mergeCell ref="AD4:AF4"/>
   </mergeCells>
-  <dataValidations count="17">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:C12 B13:D70" type="decimal">
+  <dataValidations count="16">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:C12 B13:D70" type="decimal">
       <formula1>-277</formula1>
       <formula2>500</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D6:D12" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D6:D12" type="list">
       <formula1>"low,medium,high"</formula1>
       <formula2>500</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 E6:E14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 E6:E14" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end,Temperature at beginning,Temperature at end,Temperature+element at beginning,Temperature+element at end,Temperature+element+edge at beginning,Temperature+element+edge at "</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X6:AC6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X6:AC6" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AD6:AF6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AD6:AF6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X7:AC14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X7:AC14" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6:L14" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G14" type="whole">
+      <formula1>0</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J14" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:W6 W7:W14" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6:L14" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G14" type="whole">
-      <formula1>0</formula1>
-      <formula2>1000</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
-      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I14" type="list">
+      <formula1>"transmission,fluorescence,reference,yield,pilatus,test,"</formula1>
       <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I14" type="list">
-      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J14" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:W6 W7:W14" type="none">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -4884,10 +4883,10 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="L6" activeCellId="0" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="I12" activeCellId="0" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
@@ -4896,7 +4895,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="12.1"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="12.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="13" style="0" width="29.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="16" style="0" width="22.14"/>
@@ -4913,7 +4912,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="65" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="4"/>
@@ -4944,7 +4943,7 @@
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 14</v>
+        <v>Version: 15</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -4958,7 +4957,7 @@
       <c r="K2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="65" t="s">
+      <c r="L2" s="66" t="s">
         <v>5</v>
       </c>
       <c r="M2" s="8" t="s">
@@ -5244,24 +5243,24 @@
       <c r="F7" s="54"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="56"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="57"/>
       <c r="L7" s="52"/>
-      <c r="M7" s="57"/>
+      <c r="M7" s="58"/>
       <c r="N7" s="54"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="57"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="58"/>
       <c r="Q7" s="31"/>
-      <c r="R7" s="58"/>
-      <c r="W7" s="59"/>
-      <c r="X7" s="60"/>
-      <c r="Y7" s="61"/>
-      <c r="Z7" s="61"/>
-      <c r="AA7" s="61"/>
-      <c r="AB7" s="61"/>
-      <c r="AC7" s="62"/>
-      <c r="AD7" s="63"/>
+      <c r="R7" s="59"/>
+      <c r="W7" s="60"/>
+      <c r="X7" s="61"/>
+      <c r="Y7" s="62"/>
+      <c r="Z7" s="62"/>
+      <c r="AA7" s="62"/>
+      <c r="AB7" s="62"/>
+      <c r="AC7" s="63"/>
+      <c r="AD7" s="64"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="52" t="n">
@@ -5275,24 +5274,24 @@
       <c r="F8" s="54"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="56"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="57"/>
       <c r="L8" s="52"/>
-      <c r="M8" s="57"/>
+      <c r="M8" s="58"/>
       <c r="N8" s="54"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="57"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="58"/>
       <c r="Q8" s="31"/>
-      <c r="R8" s="58"/>
-      <c r="W8" s="59"/>
-      <c r="X8" s="60"/>
-      <c r="Y8" s="61"/>
-      <c r="Z8" s="61"/>
-      <c r="AA8" s="61"/>
-      <c r="AB8" s="61"/>
-      <c r="AC8" s="62"/>
-      <c r="AD8" s="63"/>
+      <c r="R8" s="59"/>
+      <c r="W8" s="60"/>
+      <c r="X8" s="61"/>
+      <c r="Y8" s="62"/>
+      <c r="Z8" s="62"/>
+      <c r="AA8" s="62"/>
+      <c r="AB8" s="62"/>
+      <c r="AC8" s="63"/>
+      <c r="AD8" s="64"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="52" t="n">
@@ -5306,24 +5305,24 @@
       <c r="F9" s="31"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="56"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="57"/>
       <c r="L9" s="52"/>
-      <c r="M9" s="57"/>
+      <c r="M9" s="58"/>
       <c r="N9" s="54"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="57"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="58"/>
       <c r="Q9" s="31"/>
-      <c r="R9" s="58"/>
-      <c r="W9" s="59"/>
-      <c r="X9" s="60"/>
-      <c r="Y9" s="61"/>
-      <c r="Z9" s="61"/>
-      <c r="AA9" s="61"/>
-      <c r="AB9" s="61"/>
-      <c r="AC9" s="62"/>
-      <c r="AD9" s="63"/>
+      <c r="R9" s="59"/>
+      <c r="W9" s="60"/>
+      <c r="X9" s="61"/>
+      <c r="Y9" s="62"/>
+      <c r="Z9" s="62"/>
+      <c r="AA9" s="62"/>
+      <c r="AB9" s="62"/>
+      <c r="AC9" s="63"/>
+      <c r="AD9" s="64"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="52" t="n">
@@ -5337,24 +5336,24 @@
       <c r="F10" s="31"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="56"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="57"/>
       <c r="L10" s="52"/>
-      <c r="M10" s="57"/>
+      <c r="M10" s="58"/>
       <c r="N10" s="54"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="57"/>
+      <c r="O10" s="59"/>
+      <c r="P10" s="58"/>
       <c r="Q10" s="31"/>
-      <c r="R10" s="58"/>
-      <c r="W10" s="59"/>
-      <c r="X10" s="60"/>
-      <c r="Y10" s="61"/>
-      <c r="Z10" s="61"/>
-      <c r="AA10" s="61"/>
-      <c r="AB10" s="61"/>
-      <c r="AC10" s="62"/>
-      <c r="AD10" s="63"/>
+      <c r="R10" s="59"/>
+      <c r="W10" s="60"/>
+      <c r="X10" s="61"/>
+      <c r="Y10" s="62"/>
+      <c r="Z10" s="62"/>
+      <c r="AA10" s="62"/>
+      <c r="AB10" s="62"/>
+      <c r="AC10" s="63"/>
+      <c r="AD10" s="64"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="52" t="n">
@@ -5368,24 +5367,24 @@
       <c r="F11" s="31"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="57"/>
       <c r="L11" s="52"/>
-      <c r="M11" s="57"/>
+      <c r="M11" s="58"/>
       <c r="N11" s="54"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="57"/>
+      <c r="O11" s="59"/>
+      <c r="P11" s="58"/>
       <c r="Q11" s="31"/>
-      <c r="R11" s="58"/>
-      <c r="W11" s="59"/>
-      <c r="X11" s="60"/>
-      <c r="Y11" s="61"/>
-      <c r="Z11" s="61"/>
-      <c r="AA11" s="61"/>
-      <c r="AB11" s="61"/>
-      <c r="AC11" s="62"/>
-      <c r="AD11" s="63"/>
+      <c r="R11" s="59"/>
+      <c r="W11" s="60"/>
+      <c r="X11" s="61"/>
+      <c r="Y11" s="62"/>
+      <c r="Z11" s="62"/>
+      <c r="AA11" s="62"/>
+      <c r="AB11" s="62"/>
+      <c r="AC11" s="63"/>
+      <c r="AD11" s="64"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="52" t="n">
@@ -5399,24 +5398,24 @@
       <c r="F12" s="31"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="56"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="57"/>
       <c r="L12" s="52"/>
-      <c r="M12" s="57"/>
+      <c r="M12" s="58"/>
       <c r="N12" s="54"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="57"/>
+      <c r="O12" s="59"/>
+      <c r="P12" s="58"/>
       <c r="Q12" s="31"/>
-      <c r="R12" s="58"/>
-      <c r="W12" s="59"/>
-      <c r="X12" s="60"/>
-      <c r="Y12" s="61"/>
-      <c r="Z12" s="61"/>
-      <c r="AA12" s="61"/>
-      <c r="AB12" s="61"/>
-      <c r="AC12" s="62"/>
-      <c r="AD12" s="63"/>
+      <c r="R12" s="59"/>
+      <c r="W12" s="60"/>
+      <c r="X12" s="61"/>
+      <c r="Y12" s="62"/>
+      <c r="Z12" s="62"/>
+      <c r="AA12" s="62"/>
+      <c r="AB12" s="62"/>
+      <c r="AC12" s="63"/>
+      <c r="AD12" s="64"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="52" t="n">
@@ -5430,24 +5429,24 @@
       <c r="F13" s="31"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="56"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="52"/>
-      <c r="M13" s="57"/>
+      <c r="M13" s="58"/>
       <c r="N13" s="54"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="57"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="58"/>
       <c r="Q13" s="31"/>
-      <c r="R13" s="58"/>
-      <c r="W13" s="59"/>
-      <c r="X13" s="60"/>
-      <c r="Y13" s="61"/>
-      <c r="Z13" s="61"/>
-      <c r="AA13" s="61"/>
-      <c r="AB13" s="61"/>
-      <c r="AC13" s="62"/>
-      <c r="AD13" s="63"/>
+      <c r="R13" s="59"/>
+      <c r="W13" s="60"/>
+      <c r="X13" s="61"/>
+      <c r="Y13" s="62"/>
+      <c r="Z13" s="62"/>
+      <c r="AA13" s="62"/>
+      <c r="AB13" s="62"/>
+      <c r="AC13" s="63"/>
+      <c r="AD13" s="64"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="52" t="n">
@@ -5461,24 +5460,24 @@
       <c r="F14" s="31"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="56"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="57"/>
       <c r="L14" s="52"/>
-      <c r="M14" s="57"/>
+      <c r="M14" s="58"/>
       <c r="N14" s="54"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="57"/>
+      <c r="O14" s="59"/>
+      <c r="P14" s="58"/>
       <c r="Q14" s="31"/>
-      <c r="R14" s="58"/>
-      <c r="W14" s="59"/>
-      <c r="X14" s="60"/>
-      <c r="Y14" s="61"/>
-      <c r="Z14" s="61"/>
-      <c r="AA14" s="61"/>
-      <c r="AB14" s="61"/>
-      <c r="AC14" s="62"/>
-      <c r="AD14" s="63"/>
+      <c r="R14" s="59"/>
+      <c r="W14" s="60"/>
+      <c r="X14" s="61"/>
+      <c r="Y14" s="62"/>
+      <c r="Z14" s="62"/>
+      <c r="AA14" s="62"/>
+      <c r="AB14" s="62"/>
+      <c r="AC14" s="63"/>
+      <c r="AD14" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -5494,79 +5493,75 @@
     <mergeCell ref="X4:AC4"/>
     <mergeCell ref="AD4:AF4"/>
   </mergeCells>
-  <dataValidations count="17">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:C12 B13:D70" type="decimal">
+  <dataValidations count="16">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:C12 B13:D70" type="decimal">
       <formula1>-277</formula1>
       <formula2>500</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D6:D12" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D6:D12" type="list">
       <formula1>"low,medium,high"</formula1>
       <formula2>500</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 E6:E14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 E6:E14" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end,Temperature at beginning,Temperature at end,Temperature+element at beginning,Temperature+element at end,Temperature+element+edge at beginning,Temperature+element+edge at "</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X6:AC6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X6:AC6" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AD6:AF6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AD6:AF6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X7:AC14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X7:AC14" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6:L14" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G14" type="whole">
+      <formula1>0</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J14" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:W6 W7:W14" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6:L14" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G14" type="whole">
-      <formula1>0</formula1>
-      <formula2>1000</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
-      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I14" type="list">
+      <formula1>"transmission,fluorescence,reference,yield,pilatus,test,"</formula1>
       <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I14" type="list">
-      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J14" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:W6 W7:W14" type="none">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -5583,15 +5578,15 @@
   </sheetPr>
   <dimension ref="B1:AF14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="6" ySplit="6" topLeftCell="G7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
       <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="L6" activeCellId="0" sqref="L6"/>
+      <selection pane="bottomRight" activeCell="I7" activeCellId="0" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.1"/>
@@ -5617,7 +5612,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="65" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="4"/>
@@ -5648,7 +5643,7 @@
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6" t="str">
         <f aca="false">_xlfn.CONCAT("Version: ",'Version history'!A3)</f>
-        <v>Version: 14</v>
+        <v>Version: 15</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="7"/>
@@ -5662,7 +5657,7 @@
       <c r="K2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="L2" s="65" t="s">
+      <c r="L2" s="66" t="s">
         <v>5</v>
       </c>
       <c r="M2" s="8" t="s">
@@ -5948,24 +5943,24 @@
       <c r="F7" s="54"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="56"/>
+      <c r="I7" s="55"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="57"/>
       <c r="L7" s="52"/>
-      <c r="M7" s="57"/>
+      <c r="M7" s="58"/>
       <c r="N7" s="54"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="57"/>
+      <c r="O7" s="59"/>
+      <c r="P7" s="58"/>
       <c r="Q7" s="31"/>
-      <c r="R7" s="58"/>
-      <c r="W7" s="59"/>
-      <c r="X7" s="60"/>
-      <c r="Y7" s="61"/>
-      <c r="Z7" s="61"/>
-      <c r="AA7" s="61"/>
-      <c r="AB7" s="61"/>
-      <c r="AC7" s="62"/>
-      <c r="AD7" s="63"/>
+      <c r="R7" s="59"/>
+      <c r="W7" s="60"/>
+      <c r="X7" s="61"/>
+      <c r="Y7" s="62"/>
+      <c r="Z7" s="62"/>
+      <c r="AA7" s="62"/>
+      <c r="AB7" s="62"/>
+      <c r="AC7" s="63"/>
+      <c r="AD7" s="64"/>
     </row>
     <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="52" t="n">
@@ -5979,24 +5974,24 @@
       <c r="F8" s="54"/>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="55"/>
-      <c r="K8" s="56"/>
+      <c r="I8" s="55"/>
+      <c r="J8" s="56"/>
+      <c r="K8" s="57"/>
       <c r="L8" s="52"/>
-      <c r="M8" s="57"/>
+      <c r="M8" s="58"/>
       <c r="N8" s="54"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="57"/>
+      <c r="O8" s="59"/>
+      <c r="P8" s="58"/>
       <c r="Q8" s="31"/>
-      <c r="R8" s="58"/>
-      <c r="W8" s="59"/>
-      <c r="X8" s="60"/>
-      <c r="Y8" s="61"/>
-      <c r="Z8" s="61"/>
-      <c r="AA8" s="61"/>
-      <c r="AB8" s="61"/>
-      <c r="AC8" s="62"/>
-      <c r="AD8" s="63"/>
+      <c r="R8" s="59"/>
+      <c r="W8" s="60"/>
+      <c r="X8" s="61"/>
+      <c r="Y8" s="62"/>
+      <c r="Z8" s="62"/>
+      <c r="AA8" s="62"/>
+      <c r="AB8" s="62"/>
+      <c r="AC8" s="63"/>
+      <c r="AD8" s="64"/>
     </row>
     <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="52" t="n">
@@ -6010,24 +6005,24 @@
       <c r="F9" s="31"/>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="55"/>
-      <c r="K9" s="56"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="56"/>
+      <c r="K9" s="57"/>
       <c r="L9" s="52"/>
-      <c r="M9" s="57"/>
+      <c r="M9" s="58"/>
       <c r="N9" s="54"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="57"/>
+      <c r="O9" s="59"/>
+      <c r="P9" s="58"/>
       <c r="Q9" s="31"/>
-      <c r="R9" s="58"/>
-      <c r="W9" s="59"/>
-      <c r="X9" s="60"/>
-      <c r="Y9" s="61"/>
-      <c r="Z9" s="61"/>
-      <c r="AA9" s="61"/>
-      <c r="AB9" s="61"/>
-      <c r="AC9" s="62"/>
-      <c r="AD9" s="63"/>
+      <c r="R9" s="59"/>
+      <c r="W9" s="60"/>
+      <c r="X9" s="61"/>
+      <c r="Y9" s="62"/>
+      <c r="Z9" s="62"/>
+      <c r="AA9" s="62"/>
+      <c r="AB9" s="62"/>
+      <c r="AC9" s="63"/>
+      <c r="AD9" s="64"/>
     </row>
     <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="52" t="n">
@@ -6041,24 +6036,24 @@
       <c r="F10" s="31"/>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="55"/>
-      <c r="K10" s="56"/>
+      <c r="I10" s="55"/>
+      <c r="J10" s="56"/>
+      <c r="K10" s="57"/>
       <c r="L10" s="52"/>
-      <c r="M10" s="57"/>
+      <c r="M10" s="58"/>
       <c r="N10" s="54"/>
-      <c r="O10" s="58"/>
-      <c r="P10" s="57"/>
+      <c r="O10" s="59"/>
+      <c r="P10" s="58"/>
       <c r="Q10" s="31"/>
-      <c r="R10" s="58"/>
-      <c r="W10" s="59"/>
-      <c r="X10" s="60"/>
-      <c r="Y10" s="61"/>
-      <c r="Z10" s="61"/>
-      <c r="AA10" s="61"/>
-      <c r="AB10" s="61"/>
-      <c r="AC10" s="62"/>
-      <c r="AD10" s="63"/>
+      <c r="R10" s="59"/>
+      <c r="W10" s="60"/>
+      <c r="X10" s="61"/>
+      <c r="Y10" s="62"/>
+      <c r="Z10" s="62"/>
+      <c r="AA10" s="62"/>
+      <c r="AB10" s="62"/>
+      <c r="AC10" s="63"/>
+      <c r="AD10" s="64"/>
     </row>
     <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="52" t="n">
@@ -6072,24 +6067,24 @@
       <c r="F11" s="31"/>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="55"/>
-      <c r="K11" s="56"/>
+      <c r="I11" s="55"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="57"/>
       <c r="L11" s="52"/>
-      <c r="M11" s="57"/>
+      <c r="M11" s="58"/>
       <c r="N11" s="54"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="57"/>
+      <c r="O11" s="59"/>
+      <c r="P11" s="58"/>
       <c r="Q11" s="31"/>
-      <c r="R11" s="58"/>
-      <c r="W11" s="59"/>
-      <c r="X11" s="60"/>
-      <c r="Y11" s="61"/>
-      <c r="Z11" s="61"/>
-      <c r="AA11" s="61"/>
-      <c r="AB11" s="61"/>
-      <c r="AC11" s="62"/>
-      <c r="AD11" s="63"/>
+      <c r="R11" s="59"/>
+      <c r="W11" s="60"/>
+      <c r="X11" s="61"/>
+      <c r="Y11" s="62"/>
+      <c r="Z11" s="62"/>
+      <c r="AA11" s="62"/>
+      <c r="AB11" s="62"/>
+      <c r="AC11" s="63"/>
+      <c r="AD11" s="64"/>
     </row>
     <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="52" t="n">
@@ -6103,24 +6098,24 @@
       <c r="F12" s="31"/>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="55"/>
-      <c r="K12" s="56"/>
+      <c r="I12" s="55"/>
+      <c r="J12" s="56"/>
+      <c r="K12" s="57"/>
       <c r="L12" s="52"/>
-      <c r="M12" s="57"/>
+      <c r="M12" s="58"/>
       <c r="N12" s="54"/>
-      <c r="O12" s="58"/>
-      <c r="P12" s="57"/>
+      <c r="O12" s="59"/>
+      <c r="P12" s="58"/>
       <c r="Q12" s="31"/>
-      <c r="R12" s="58"/>
-      <c r="W12" s="59"/>
-      <c r="X12" s="60"/>
-      <c r="Y12" s="61"/>
-      <c r="Z12" s="61"/>
-      <c r="AA12" s="61"/>
-      <c r="AB12" s="61"/>
-      <c r="AC12" s="62"/>
-      <c r="AD12" s="63"/>
+      <c r="R12" s="59"/>
+      <c r="W12" s="60"/>
+      <c r="X12" s="61"/>
+      <c r="Y12" s="62"/>
+      <c r="Z12" s="62"/>
+      <c r="AA12" s="62"/>
+      <c r="AB12" s="62"/>
+      <c r="AC12" s="63"/>
+      <c r="AD12" s="64"/>
     </row>
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B13" s="52" t="n">
@@ -6134,24 +6129,24 @@
       <c r="F13" s="31"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
-      <c r="I13" s="14"/>
-      <c r="J13" s="55"/>
-      <c r="K13" s="56"/>
+      <c r="I13" s="55"/>
+      <c r="J13" s="56"/>
+      <c r="K13" s="57"/>
       <c r="L13" s="52"/>
-      <c r="M13" s="57"/>
+      <c r="M13" s="58"/>
       <c r="N13" s="54"/>
-      <c r="O13" s="58"/>
-      <c r="P13" s="57"/>
+      <c r="O13" s="59"/>
+      <c r="P13" s="58"/>
       <c r="Q13" s="31"/>
-      <c r="R13" s="58"/>
-      <c r="W13" s="59"/>
-      <c r="X13" s="60"/>
-      <c r="Y13" s="61"/>
-      <c r="Z13" s="61"/>
-      <c r="AA13" s="61"/>
-      <c r="AB13" s="61"/>
-      <c r="AC13" s="62"/>
-      <c r="AD13" s="63"/>
+      <c r="R13" s="59"/>
+      <c r="W13" s="60"/>
+      <c r="X13" s="61"/>
+      <c r="Y13" s="62"/>
+      <c r="Z13" s="62"/>
+      <c r="AA13" s="62"/>
+      <c r="AB13" s="62"/>
+      <c r="AC13" s="63"/>
+      <c r="AD13" s="64"/>
     </row>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="52" t="n">
@@ -6165,24 +6160,24 @@
       <c r="F14" s="31"/>
       <c r="G14" s="14"/>
       <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="56"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="56"/>
+      <c r="K14" s="57"/>
       <c r="L14" s="52"/>
-      <c r="M14" s="57"/>
+      <c r="M14" s="58"/>
       <c r="N14" s="54"/>
-      <c r="O14" s="58"/>
-      <c r="P14" s="57"/>
+      <c r="O14" s="59"/>
+      <c r="P14" s="58"/>
       <c r="Q14" s="31"/>
-      <c r="R14" s="58"/>
-      <c r="W14" s="59"/>
-      <c r="X14" s="60"/>
-      <c r="Y14" s="61"/>
-      <c r="Z14" s="61"/>
-      <c r="AA14" s="61"/>
-      <c r="AB14" s="61"/>
-      <c r="AC14" s="62"/>
-      <c r="AD14" s="63"/>
+      <c r="R14" s="59"/>
+      <c r="W14" s="60"/>
+      <c r="X14" s="61"/>
+      <c r="Y14" s="62"/>
+      <c r="Z14" s="62"/>
+      <c r="AA14" s="62"/>
+      <c r="AB14" s="62"/>
+      <c r="AC14" s="63"/>
+      <c r="AD14" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -6198,79 +6193,75 @@
     <mergeCell ref="X4:AC4"/>
     <mergeCell ref="AD4:AF4"/>
   </mergeCells>
-  <dataValidations count="17">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:C12 B13:D70" type="decimal">
+  <dataValidations count="16">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B7:C12 B13:D70" type="decimal">
       <formula1>-277</formula1>
       <formula2>500</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D6:D12" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="D6:D12" type="list">
       <formula1>"low,medium,high"</formula1>
       <formula2>500</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 E6:E14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J2 E6:E14" type="list">
       <formula1>"Yes,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L2" type="list">
       <formula1>"No,Element at beginning,Element at end,Element+edge at beginning,Element+edge at end,Temperature at beginning,Temperature at end,Temperature+element at beginning,Temperature+element at end,Temperature+element+edge at beginning,Temperature+element+edge at "</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
+    <dataValidation allowBlank="true" operator="greaterThanOrEqual" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="N2" type="whole">
       <formula1>1</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X6:AC6" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X6:AC6" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AD6:AF6" type="decimal">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="AD6:AF6" type="decimal">
       <formula1>-0.1</formula1>
       <formula2>8</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X7:AC14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="X7:AC14" type="list">
       <formula1>"True,False"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="K6:K14" type="list">
       <formula1>"K,L3,L2,L1"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6:L14" type="list">
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G14" type="whole">
+      <formula1>0</formula1>
+      <formula2>1000</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J14" type="list">
+      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:W6 W7:W14" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
+      <formula1>10</formula1>
+      <formula2>210</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="L6:L14" type="list">
       <formula1>"unfocused,focused"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="G6:G14" type="whole">
-      <formula1>0</formula1>
-      <formula2>1000</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6" type="list">
-      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I6:I14" type="list">
+      <formula1>"transmission,fluorescence,reference,yield,pilatus,test,"</formula1>
       <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="I7:I14" type="list">
-      <formula1>"transmission,fluorescence,both,reference,yield,test,xs"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J6" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="J7:J14" type="list">
-      <formula1>"Ca,Sc,Ti,V,Cr,Mn,Fe,Co,Ni,Cu,Zn,Ga,Ge,As,Se,Br,Kr,Rb,Sr,Y,Zr,Nb,Mo,Tc,Ru,Pd,Ag,Cd,In,Sn,Sb,Te,I,Xe,Cs,Ba,La,Ce,Pr,Nd,Pm,Sm,Eu,Gd,Tb,Dy,Ho,Er,Tm,Yb,Lu,Hf,Ta,W,Re,Os,Ir,Pt,Au,Hg,Tl,Pb,Bi,Po,At,Rn,Fr,Ra,Ac,Th,Pa,U,Np,Pu,Am"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="V6:W6 W7:W14" type="none">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
-    </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="S6:U6" type="none">
-      <formula1>10</formula1>
-      <formula2>210</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -6285,41 +6276,41 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="1" sqref="L6 B19"/>
+      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="115.2"/>
   </cols>
   <sheetData>
-    <row r="1" s="66" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="67" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="30" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" s="66" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="67" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="30" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="3" s="66" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" s="67" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="30" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" s="66" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" s="67" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="30"/>
     </row>
-    <row r="5" s="66" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="67" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="66" t="s">
+      <c r="B5" s="67" t="s">
         <v>61</v>
       </c>
     </row>
@@ -6423,7 +6414,7 @@
       <c r="A18" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B18" s="67" t="s">
+      <c r="B18" s="68" t="s">
         <v>74</v>
       </c>
     </row>
@@ -6435,10 +6426,18 @@
         <v>75</v>
       </c>
     </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>